<commit_message>
Changed filenames and paths for clarity
</commit_message>
<xml_diff>
--- a/Documents/CubeSatTeamRoster.xlsx
+++ b/Documents/CubeSatTeamRoster.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JustinSeif\Documents\GitHub\CubeSat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles\Desktop\CubeSat\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24120" windowHeight="13404"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24120" windowHeight="13410"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>Charles Denis</t>
   </si>
@@ -132,6 +132,12 @@
   </si>
   <si>
     <t>Power</t>
+  </si>
+  <si>
+    <t>ADNCS</t>
+  </si>
+  <si>
+    <t>Power systems</t>
   </si>
 </sst>
 </file>
@@ -201,7 +207,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -229,6 +235,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -514,23 +523,23 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="25.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.44140625" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" customWidth="1"/>
-    <col min="4" max="4" width="25.33203125" style="9"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="5" t="s">
         <v>30</v>
       </c>
       <c r="D1" s="8"/>
     </row>
-    <row r="2" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>27</v>
       </c>
@@ -544,7 +553,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -558,7 +567,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -568,8 +577,11 @@
       <c r="C4" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D4" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -583,7 +595,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -593,8 +605,11 @@
       <c r="C6" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D6" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -608,7 +623,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -618,8 +633,11 @@
       <c r="C8" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D8" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -629,8 +647,11 @@
       <c r="C9" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D9" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -640,8 +661,11 @@
       <c r="C10" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D10" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -651,52 +675,55 @@
       <c r="C11" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D11" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C23" s="2"/>
     </row>
   </sheetData>
@@ -712,7 +739,7 @@
     <hyperlink ref="B11" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Updated PDR first few slides
</commit_message>
<xml_diff>
--- a/Documents/CubeSatTeamRoster.xlsx
+++ b/Documents/CubeSatTeamRoster.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
   <si>
     <t>Charles Denis</t>
   </si>
@@ -135,9 +135,6 @@
   </si>
   <si>
     <t>ADNCS</t>
-  </si>
-  <si>
-    <t>Power systems</t>
   </si>
 </sst>
 </file>
@@ -523,7 +520,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,7 +631,7 @@
         <v>13</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>